<commit_message>
modelo mejorado con gemini
</commit_message>
<xml_diff>
--- a/historicoquiniela.xlsx
+++ b/historicoquiniela.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="49">
   <si>
     <t>Zamuro</t>
   </si>
@@ -557,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AFI163"/>
+  <dimension ref="A1:AFN163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AEP1" workbookViewId="0">
-      <selection activeCell="AFK2" sqref="AFK2:AFK7"/>
+    <sheetView tabSelected="1" topLeftCell="AET1" workbookViewId="0">
+      <selection activeCell="AFN2" sqref="AFN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -577,9 +577,12 @@
     <col min="838" max="838" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="839" max="839" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="840" max="840" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="842" max="842" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="843" max="843" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="845" max="845" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:841">
+    <row r="1" spans="1:846">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -3103,8 +3106,23 @@
       <c r="AFI1" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="AFJ1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AFK1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AFL1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AFM1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AFN1" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:841">
+    <row r="2" spans="1:846">
       <c r="A2">
         <v>10</v>
       </c>
@@ -5625,8 +5643,20 @@
       <c r="AFI2" s="8">
         <v>12</v>
       </c>
+      <c r="AFJ2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AFK2" s="8">
+        <v>8</v>
+      </c>
+      <c r="AFL2" s="8">
+        <v>9</v>
+      </c>
+      <c r="AFM2" s="8">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:841">
+    <row r="3" spans="1:846">
       <c r="A3">
         <v>11</v>
       </c>
@@ -8147,8 +8177,20 @@
       <c r="AFI3">
         <v>16</v>
       </c>
+      <c r="AFJ3">
+        <v>4</v>
+      </c>
+      <c r="AFK3">
+        <v>15</v>
+      </c>
+      <c r="AFL3">
+        <v>22</v>
+      </c>
+      <c r="AFM3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:841">
+    <row r="4" spans="1:846">
       <c r="A4">
         <v>12</v>
       </c>
@@ -10669,8 +10711,20 @@
       <c r="AFI4">
         <v>17</v>
       </c>
+      <c r="AFJ4">
+        <v>7</v>
+      </c>
+      <c r="AFK4">
+        <v>18</v>
+      </c>
+      <c r="AFL4">
+        <v>23</v>
+      </c>
+      <c r="AFM4">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:841">
+    <row r="5" spans="1:846">
       <c r="A5">
         <v>1</v>
       </c>
@@ -13191,8 +13245,20 @@
       <c r="AFI5">
         <v>23</v>
       </c>
+      <c r="AFJ5">
+        <v>10</v>
+      </c>
+      <c r="AFK5">
+        <v>21</v>
+      </c>
+      <c r="AFL5">
+        <v>24</v>
+      </c>
+      <c r="AFM5">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:841">
+    <row r="6" spans="1:846">
       <c r="A6">
         <v>2</v>
       </c>
@@ -15713,8 +15779,20 @@
       <c r="AFI6">
         <v>31</v>
       </c>
+      <c r="AFJ6">
+        <v>24</v>
+      </c>
+      <c r="AFK6">
+        <v>28</v>
+      </c>
+      <c r="AFL6">
+        <v>26</v>
+      </c>
+      <c r="AFM6">
+        <v>32</v>
+      </c>
     </row>
-    <row r="7" spans="1:841">
+    <row r="7" spans="1:846">
       <c r="A7">
         <v>3</v>
       </c>
@@ -18235,15 +18313,27 @@
       <c r="AFI7">
         <v>32</v>
       </c>
+      <c r="AFJ7">
+        <v>29</v>
+      </c>
+      <c r="AFK7">
+        <v>35</v>
+      </c>
+      <c r="AFL7">
+        <v>29</v>
+      </c>
+      <c r="AFM7">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:841">
+    <row r="8" spans="1:846">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:841">
+    <row r="9" spans="1:846">
       <c r="NI9" s="2"/>
       <c r="NJ9" s="2"/>
     </row>
-    <row r="14" spans="1:841">
+    <row r="14" spans="1:846">
       <c r="AEG14">
         <f>100+38+9+9+15+50</f>
         <v>221</v>

</xml_diff>

<commit_message>
se agrego modelo con persistencia
</commit_message>
<xml_diff>
--- a/historicoquiniela.xlsx
+++ b/historicoquiniela.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Dropbox\python y flask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA36C82-6668-40F4-A921-64636BDE55A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F96432-F248-4434-A609-ABE003E24E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="14400" windowHeight="7335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="52">
   <si>
     <t>Zamuro</t>
   </si>
@@ -584,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AKQ162"/>
+  <dimension ref="A1:AKS162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AKA1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AKQ7" sqref="AKQ7"/>
+      <selection activeCell="AKS7" sqref="AKS7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +616,7 @@
     <col min="974" max="974" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:979" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:981" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10</v>
       </c>
@@ -3551,8 +3551,14 @@
       <c r="AKQ1">
         <v>0</v>
       </c>
+      <c r="AKR1">
+        <v>10</v>
+      </c>
+      <c r="AKS1">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:979" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:981" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -6487,8 +6493,14 @@
       <c r="AKQ2">
         <v>4</v>
       </c>
+      <c r="AKR2">
+        <v>15</v>
+      </c>
+      <c r="AKS2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:979" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:981" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -9423,8 +9435,14 @@
       <c r="AKQ3">
         <v>6</v>
       </c>
+      <c r="AKR3">
+        <v>16</v>
+      </c>
+      <c r="AKS3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:979" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:981" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -12359,8 +12377,14 @@
       <c r="AKQ4">
         <v>17</v>
       </c>
+      <c r="AKR4">
+        <v>20</v>
+      </c>
+      <c r="AKS4">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:979" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:981" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14</v>
       </c>
@@ -15295,8 +15319,14 @@
       <c r="AKQ5">
         <v>28</v>
       </c>
+      <c r="AKR5">
+        <v>23</v>
+      </c>
+      <c r="AKS5">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:979" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:981" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -18231,16 +18261,22 @@
       <c r="AKQ6">
         <v>34</v>
       </c>
+      <c r="AKR6">
+        <v>25</v>
+      </c>
+      <c r="AKS6">
+        <v>36</v>
+      </c>
     </row>
-    <row r="7" spans="1:979" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:981" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="AFP7" s="6"/>
     </row>
-    <row r="8" spans="1:979" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:981" x14ac:dyDescent="0.25">
       <c r="NI8" s="2"/>
       <c r="NJ8" s="2"/>
     </row>
-    <row r="9" spans="1:979" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:981" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>45</v>
       </c>
@@ -21174,6 +21210,12 @@
       </c>
       <c r="AKQ9" s="5" t="s">
         <v>49</v>
+      </c>
+      <c r="AKR9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AKS9" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="373:661" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
otras mejoreas al modelo Balancear entre números de alta confianza y diversificación
</commit_message>
<xml_diff>
--- a/historicoquiniela.xlsx
+++ b/historicoquiniela.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Dropbox\python y flask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACC3510-1F8F-465A-A0A4-C546A9769A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D995BDEC-FA5E-483E-913B-26473FB43BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="52">
   <si>
     <t>Zamuro</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMH162"/>
+  <dimension ref="A1:AML162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ALI1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AMH7" sqref="AMH7"/>
+    <sheetView tabSelected="1" topLeftCell="ALN1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AML7" sqref="AML7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
     <col min="974" max="974" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10</v>
       </c>
@@ -3688,8 +3688,20 @@
       <c r="AMH1">
         <v>5</v>
       </c>
+      <c r="AMI1">
+        <v>3</v>
+      </c>
+      <c r="AMJ1">
+        <v>1</v>
+      </c>
+      <c r="AMK1">
+        <v>0</v>
+      </c>
+      <c r="AML1">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -6753,8 +6765,20 @@
       <c r="AMH2">
         <v>13</v>
       </c>
+      <c r="AMI2">
+        <v>13</v>
+      </c>
+      <c r="AMJ2">
+        <v>7</v>
+      </c>
+      <c r="AMK2">
+        <v>5</v>
+      </c>
+      <c r="AML2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -9818,8 +9842,20 @@
       <c r="AMH3">
         <v>31</v>
       </c>
+      <c r="AMI3">
+        <v>15</v>
+      </c>
+      <c r="AMJ3">
+        <v>11</v>
+      </c>
+      <c r="AMK3">
+        <v>6</v>
+      </c>
+      <c r="AML3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -12883,8 +12919,20 @@
       <c r="AMH4">
         <v>32</v>
       </c>
+      <c r="AMI4">
+        <v>19</v>
+      </c>
+      <c r="AMJ4">
+        <v>20</v>
+      </c>
+      <c r="AMK4">
+        <v>12</v>
+      </c>
+      <c r="AML4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14</v>
       </c>
@@ -15948,8 +15996,20 @@
       <c r="AMH5">
         <v>15</v>
       </c>
+      <c r="AMI5">
+        <v>32</v>
+      </c>
+      <c r="AMJ5">
+        <v>22</v>
+      </c>
+      <c r="AMK5">
+        <v>20</v>
+      </c>
+      <c r="AML5">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -19013,16 +19073,28 @@
       <c r="AMH6">
         <v>36</v>
       </c>
+      <c r="AMI6">
+        <v>36</v>
+      </c>
+      <c r="AMJ6">
+        <v>31</v>
+      </c>
+      <c r="AMK6">
+        <v>30</v>
+      </c>
+      <c r="AML6">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="AFP7" s="6"/>
     </row>
-    <row r="8" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="NI8" s="2"/>
       <c r="NJ8" s="2"/>
     </row>
-    <row r="9" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>45</v>
       </c>
@@ -22085,6 +22157,18 @@
       </c>
       <c r="AMH9" s="5" t="s">
         <v>50</v>
+      </c>
+      <c r="AMI9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AMJ9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AMK9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AML9" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="373:661" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
scritp que busca patrones por dia seleccionado
</commit_message>
<xml_diff>
--- a/historicoquiniela.xlsx
+++ b/historicoquiniela.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Dropbox\python y flask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D995BDEC-FA5E-483E-913B-26473FB43BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECC4BA9-35F9-478F-BF47-CD243DBBBEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="52">
   <si>
     <t>Zamuro</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AML162"/>
+  <dimension ref="A1:ANE162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ALN1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AML7" sqref="AML7"/>
+    <sheetView tabSelected="1" topLeftCell="AML1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="ANE7" sqref="ANE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
     <col min="974" max="974" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1045" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10</v>
       </c>
@@ -3700,8 +3700,65 @@
       <c r="AML1">
         <v>8</v>
       </c>
+      <c r="AMM1">
+        <v>4</v>
+      </c>
+      <c r="AMN1">
+        <v>0</v>
+      </c>
+      <c r="AMO1">
+        <v>0</v>
+      </c>
+      <c r="AMP1">
+        <v>0</v>
+      </c>
+      <c r="AMQ1">
+        <v>12</v>
+      </c>
+      <c r="AMR1">
+        <v>1</v>
+      </c>
+      <c r="AMS1">
+        <v>6</v>
+      </c>
+      <c r="AMT1">
+        <v>0</v>
+      </c>
+      <c r="AMU1">
+        <v>1</v>
+      </c>
+      <c r="AMV1">
+        <v>0</v>
+      </c>
+      <c r="AMW1">
+        <v>20</v>
+      </c>
+      <c r="AMX1">
+        <v>20</v>
+      </c>
+      <c r="AMY1">
+        <v>3</v>
+      </c>
+      <c r="AMZ1">
+        <v>14</v>
+      </c>
+      <c r="ANA1">
+        <v>0</v>
+      </c>
+      <c r="ANB1">
+        <v>0</v>
+      </c>
+      <c r="ANC1">
+        <v>7</v>
+      </c>
+      <c r="AND1">
+        <v>0</v>
+      </c>
+      <c r="ANE1">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1045" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -6777,8 +6834,65 @@
       <c r="AML2">
         <v>11</v>
       </c>
+      <c r="AMM2">
+        <v>10</v>
+      </c>
+      <c r="AMN2">
+        <v>4</v>
+      </c>
+      <c r="AMO2">
+        <v>2</v>
+      </c>
+      <c r="AMP2">
+        <v>7</v>
+      </c>
+      <c r="AMQ2">
+        <v>13</v>
+      </c>
+      <c r="AMR2">
+        <v>9</v>
+      </c>
+      <c r="AMS2">
+        <v>7</v>
+      </c>
+      <c r="AMT2">
+        <v>10</v>
+      </c>
+      <c r="AMU2">
+        <v>9</v>
+      </c>
+      <c r="AMV2">
+        <v>8</v>
+      </c>
+      <c r="AMW2">
+        <v>22</v>
+      </c>
+      <c r="AMX2">
+        <v>25</v>
+      </c>
+      <c r="AMY2">
+        <v>18</v>
+      </c>
+      <c r="AMZ2">
+        <v>20</v>
+      </c>
+      <c r="ANA2">
+        <v>0</v>
+      </c>
+      <c r="ANB2">
+        <v>11</v>
+      </c>
+      <c r="ANC2">
+        <v>8</v>
+      </c>
+      <c r="AND2">
+        <v>3</v>
+      </c>
+      <c r="ANE2">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1045" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -9854,8 +9968,65 @@
       <c r="AML3">
         <v>12</v>
       </c>
+      <c r="AMM3">
+        <v>19</v>
+      </c>
+      <c r="AMN3">
+        <v>9</v>
+      </c>
+      <c r="AMO3">
+        <v>11</v>
+      </c>
+      <c r="AMP3">
+        <v>15</v>
+      </c>
+      <c r="AMQ3">
+        <v>15</v>
+      </c>
+      <c r="AMR3">
+        <v>16</v>
+      </c>
+      <c r="AMS3">
+        <v>8</v>
+      </c>
+      <c r="AMT3">
+        <v>11</v>
+      </c>
+      <c r="AMU3">
+        <v>14</v>
+      </c>
+      <c r="AMV3">
+        <v>24</v>
+      </c>
+      <c r="AMW3">
+        <v>24</v>
+      </c>
+      <c r="AMX3">
+        <v>33</v>
+      </c>
+      <c r="AMY3">
+        <v>10</v>
+      </c>
+      <c r="AMZ3">
+        <v>26</v>
+      </c>
+      <c r="ANA3">
+        <v>22</v>
+      </c>
+      <c r="ANB3">
+        <v>14</v>
+      </c>
+      <c r="ANC3">
+        <v>16</v>
+      </c>
+      <c r="AND3">
+        <v>8</v>
+      </c>
+      <c r="ANE3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1045" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -12931,8 +13102,65 @@
       <c r="AML4">
         <v>14</v>
       </c>
+      <c r="AMM4">
+        <v>25</v>
+      </c>
+      <c r="AMN4">
+        <v>13</v>
+      </c>
+      <c r="AMO4">
+        <v>16</v>
+      </c>
+      <c r="AMP4">
+        <v>13</v>
+      </c>
+      <c r="AMQ4">
+        <v>23</v>
+      </c>
+      <c r="AMR4">
+        <v>28</v>
+      </c>
+      <c r="AMS4">
+        <v>20</v>
+      </c>
+      <c r="AMT4">
+        <v>13</v>
+      </c>
+      <c r="AMU4">
+        <v>18</v>
+      </c>
+      <c r="AMV4">
+        <v>25</v>
+      </c>
+      <c r="AMW4">
+        <v>25</v>
+      </c>
+      <c r="AMX4">
+        <v>34</v>
+      </c>
+      <c r="AMY4">
+        <v>20</v>
+      </c>
+      <c r="AMZ4">
+        <v>27</v>
+      </c>
+      <c r="ANA4">
+        <v>23</v>
+      </c>
+      <c r="ANB4">
+        <v>23</v>
+      </c>
+      <c r="ANC4">
+        <v>26</v>
+      </c>
+      <c r="AND4">
+        <v>11</v>
+      </c>
+      <c r="ANE4">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1045" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14</v>
       </c>
@@ -16008,8 +16236,65 @@
       <c r="AML5">
         <v>15</v>
       </c>
+      <c r="AMM5">
+        <v>33</v>
+      </c>
+      <c r="AMN5">
+        <v>26</v>
+      </c>
+      <c r="AMO5">
+        <v>17</v>
+      </c>
+      <c r="AMP5">
+        <v>31</v>
+      </c>
+      <c r="AMQ5">
+        <v>28</v>
+      </c>
+      <c r="AMR5">
+        <v>29</v>
+      </c>
+      <c r="AMS5">
+        <v>21</v>
+      </c>
+      <c r="AMT5">
+        <v>32</v>
+      </c>
+      <c r="AMU5">
+        <v>30</v>
+      </c>
+      <c r="AMV5">
+        <v>33</v>
+      </c>
+      <c r="AMW5">
+        <v>27</v>
+      </c>
+      <c r="AMX5">
+        <v>35</v>
+      </c>
+      <c r="AMY5">
+        <v>22</v>
+      </c>
+      <c r="AMZ5">
+        <v>29</v>
+      </c>
+      <c r="ANA5">
+        <v>33</v>
+      </c>
+      <c r="ANB5">
+        <v>29</v>
+      </c>
+      <c r="ANC5">
+        <v>29</v>
+      </c>
+      <c r="AND5">
+        <v>24</v>
+      </c>
+      <c r="ANE5">
+        <v>31</v>
+      </c>
     </row>
-    <row r="6" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1045" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -19085,16 +19370,73 @@
       <c r="AML6">
         <v>29</v>
       </c>
+      <c r="AMM6">
+        <v>34</v>
+      </c>
+      <c r="AMN6">
+        <v>34</v>
+      </c>
+      <c r="AMO6">
+        <v>22</v>
+      </c>
+      <c r="AMP6">
+        <v>34</v>
+      </c>
+      <c r="AMQ6">
+        <v>20</v>
+      </c>
+      <c r="AMR6">
+        <v>23</v>
+      </c>
+      <c r="AMS6">
+        <v>22</v>
+      </c>
+      <c r="AMT6">
+        <v>35</v>
+      </c>
+      <c r="AMU6">
+        <v>33</v>
+      </c>
+      <c r="AMV6">
+        <v>34</v>
+      </c>
+      <c r="AMW6">
+        <v>36</v>
+      </c>
+      <c r="AMX6">
+        <v>36</v>
+      </c>
+      <c r="AMY6">
+        <v>30</v>
+      </c>
+      <c r="AMZ6">
+        <v>30</v>
+      </c>
+      <c r="ANA6">
+        <v>36</v>
+      </c>
+      <c r="ANB6">
+        <v>32</v>
+      </c>
+      <c r="ANC6">
+        <v>35</v>
+      </c>
+      <c r="AND6">
+        <v>36</v>
+      </c>
+      <c r="ANE6">
+        <v>35</v>
+      </c>
     </row>
-    <row r="7" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1045" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="AFP7" s="6"/>
     </row>
-    <row r="8" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1045" x14ac:dyDescent="0.25">
       <c r="NI8" s="2"/>
       <c r="NJ8" s="2"/>
     </row>
-    <row r="9" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1045" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>45</v>
       </c>
@@ -22169,6 +22511,63 @@
       </c>
       <c r="AML9" s="5" t="s">
         <v>47</v>
+      </c>
+      <c r="AMM9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AMN9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AMO9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AMP9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AMQ9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AMR9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AMS9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AMT9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AMU9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AMV9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AMW9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AMX9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AMY9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AMZ9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="ANA9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="ANB9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="ANC9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AND9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="ANE9" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="373:661" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se genero archivo por dias
</commit_message>
<xml_diff>
--- a/historicoquiniela.xlsx
+++ b/historicoquiniela.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Dropbox\python y flask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECC4BA9-35F9-478F-BF47-CD243DBBBEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253AC334-601B-4EDA-A655-8645FB589581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="52">
   <si>
     <t>Zamuro</t>
   </si>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ANE162"/>
+  <dimension ref="A1:ANQ162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AML1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="ANE7" sqref="ANE7"/>
+    <sheetView tabSelected="1" topLeftCell="AMS1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="ANQ7" sqref="ANQ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
     <col min="974" max="974" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1045" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1057" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10</v>
       </c>
@@ -3757,8 +3757,44 @@
       <c r="ANE1">
         <v>7</v>
       </c>
+      <c r="ANF1">
+        <v>12</v>
+      </c>
+      <c r="ANG1">
+        <v>7</v>
+      </c>
+      <c r="ANH1">
+        <v>0</v>
+      </c>
+      <c r="ANI1">
+        <v>2</v>
+      </c>
+      <c r="ANJ1">
+        <v>0</v>
+      </c>
+      <c r="ANK1">
+        <v>10</v>
+      </c>
+      <c r="ANL1">
+        <v>3</v>
+      </c>
+      <c r="ANM1">
+        <v>10</v>
+      </c>
+      <c r="ANN1">
+        <v>12</v>
+      </c>
+      <c r="ANO1">
+        <v>4</v>
+      </c>
+      <c r="ANP1">
+        <v>0</v>
+      </c>
+      <c r="ANQ1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:1045" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1057" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -6891,8 +6927,44 @@
       <c r="ANE2">
         <v>17</v>
       </c>
+      <c r="ANF2">
+        <v>20</v>
+      </c>
+      <c r="ANG2">
+        <v>20</v>
+      </c>
+      <c r="ANH2">
+        <v>12</v>
+      </c>
+      <c r="ANI2">
+        <v>5</v>
+      </c>
+      <c r="ANJ2">
+        <v>0</v>
+      </c>
+      <c r="ANK2">
+        <v>17</v>
+      </c>
+      <c r="ANL2">
+        <v>6</v>
+      </c>
+      <c r="ANM2">
+        <v>15</v>
+      </c>
+      <c r="ANN2">
+        <v>13</v>
+      </c>
+      <c r="ANO2">
+        <v>10</v>
+      </c>
+      <c r="ANP2">
+        <v>18</v>
+      </c>
+      <c r="ANQ2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:1045" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1057" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -10025,8 +10097,44 @@
       <c r="ANE3">
         <v>23</v>
       </c>
+      <c r="ANF3">
+        <v>23</v>
+      </c>
+      <c r="ANG3">
+        <v>24</v>
+      </c>
+      <c r="ANH3">
+        <v>15</v>
+      </c>
+      <c r="ANI3">
+        <v>6</v>
+      </c>
+      <c r="ANJ3">
+        <v>2</v>
+      </c>
+      <c r="ANK3">
+        <v>24</v>
+      </c>
+      <c r="ANL3">
+        <v>8</v>
+      </c>
+      <c r="ANM3">
+        <v>17</v>
+      </c>
+      <c r="ANN3">
+        <v>15</v>
+      </c>
+      <c r="ANO3">
+        <v>19</v>
+      </c>
+      <c r="ANP3">
+        <v>27</v>
+      </c>
+      <c r="ANQ3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:1045" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1057" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -13159,8 +13267,44 @@
       <c r="ANE4">
         <v>28</v>
       </c>
+      <c r="ANF4">
+        <v>29</v>
+      </c>
+      <c r="ANG4">
+        <v>29</v>
+      </c>
+      <c r="ANH4">
+        <v>21</v>
+      </c>
+      <c r="ANI4">
+        <v>8</v>
+      </c>
+      <c r="ANJ4">
+        <v>5</v>
+      </c>
+      <c r="ANK4">
+        <v>25</v>
+      </c>
+      <c r="ANL4">
+        <v>16</v>
+      </c>
+      <c r="ANM4">
+        <v>22</v>
+      </c>
+      <c r="ANN4">
+        <v>23</v>
+      </c>
+      <c r="ANO4">
+        <v>25</v>
+      </c>
+      <c r="ANP4">
+        <v>28</v>
+      </c>
+      <c r="ANQ4">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:1045" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1057" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14</v>
       </c>
@@ -16293,8 +16437,44 @@
       <c r="ANE5">
         <v>31</v>
       </c>
+      <c r="ANF5">
+        <v>31</v>
+      </c>
+      <c r="ANG5">
+        <v>31</v>
+      </c>
+      <c r="ANH5">
+        <v>28</v>
+      </c>
+      <c r="ANI5">
+        <v>9</v>
+      </c>
+      <c r="ANJ5">
+        <v>7</v>
+      </c>
+      <c r="ANK5">
+        <v>27</v>
+      </c>
+      <c r="ANL5">
+        <v>27</v>
+      </c>
+      <c r="ANM5">
+        <v>27</v>
+      </c>
+      <c r="ANN5">
+        <v>28</v>
+      </c>
+      <c r="ANO5">
+        <v>33</v>
+      </c>
+      <c r="ANP5">
+        <v>32</v>
+      </c>
+      <c r="ANQ5">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:1045" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1057" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -19427,16 +19607,52 @@
       <c r="ANE6">
         <v>35</v>
       </c>
+      <c r="ANF6">
+        <v>35</v>
+      </c>
+      <c r="ANG6">
+        <v>36</v>
+      </c>
+      <c r="ANH6">
+        <v>34</v>
+      </c>
+      <c r="ANI6">
+        <v>24</v>
+      </c>
+      <c r="ANJ6">
+        <v>27</v>
+      </c>
+      <c r="ANK6">
+        <v>30</v>
+      </c>
+      <c r="ANL6">
+        <v>30</v>
+      </c>
+      <c r="ANM6">
+        <v>36</v>
+      </c>
+      <c r="ANN6">
+        <v>20</v>
+      </c>
+      <c r="ANO6">
+        <v>34</v>
+      </c>
+      <c r="ANP6">
+        <v>34</v>
+      </c>
+      <c r="ANQ6">
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="1:1045" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1057" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="AFP7" s="6"/>
     </row>
-    <row r="8" spans="1:1045" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1057" x14ac:dyDescent="0.25">
       <c r="NI8" s="2"/>
       <c r="NJ8" s="2"/>
     </row>
-    <row r="9" spans="1:1045" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1057" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>45</v>
       </c>
@@ -22568,6 +22784,42 @@
       </c>
       <c r="ANE9" s="5" t="s">
         <v>45</v>
+      </c>
+      <c r="ANF9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="ANG9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="ANH9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="ANI9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="ANJ9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="ANK9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="ANL9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="ANM9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="ANN9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="ANO9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="ANP9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="ANQ9" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="373:661" x14ac:dyDescent="0.25">

</xml_diff>